<commit_message>
Updated Data flow and drawing
</commit_message>
<xml_diff>
--- a/Detailed Design/Data Objects Table.xlsx
+++ b/Detailed Design/Data Objects Table.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="86">
   <si>
     <t>Layer</t>
   </si>
@@ -61,6 +61,219 @@
   </si>
   <si>
     <t>Print configuration data entry values</t>
+  </si>
+  <si>
+    <t>UI1</t>
+  </si>
+  <si>
+    <t>UI2</t>
+  </si>
+  <si>
+    <t>UI3</t>
+  </si>
+  <si>
+    <t>UI4</t>
+  </si>
+  <si>
+    <t>UI5</t>
+  </si>
+  <si>
+    <t>UI6</t>
+  </si>
+  <si>
+    <t>UI7</t>
+  </si>
+  <si>
+    <t>UI8</t>
+  </si>
+  <si>
+    <t>UI9</t>
+  </si>
+  <si>
+    <t>UI10</t>
+  </si>
+  <si>
+    <t>UI11</t>
+  </si>
+  <si>
+    <t>UI12</t>
+  </si>
+  <si>
+    <t>UI13</t>
+  </si>
+  <si>
+    <t>UI14</t>
+  </si>
+  <si>
+    <t>UI15</t>
+  </si>
+  <si>
+    <t>UI16</t>
+  </si>
+  <si>
+    <t>UI17</t>
+  </si>
+  <si>
+    <t>UI18</t>
+  </si>
+  <si>
+    <t>UI19</t>
+  </si>
+  <si>
+    <t>UI20</t>
+  </si>
+  <si>
+    <t>User Interface Layer</t>
+  </si>
+  <si>
+    <t>Print selections and button press</t>
+  </si>
+  <si>
+    <t>Pause, resume, and stop button Presses</t>
+  </si>
+  <si>
+    <t>Disk reads of XML and Directory structure</t>
+  </si>
+  <si>
+    <t>OI8</t>
+  </si>
+  <si>
+    <t>OI9</t>
+  </si>
+  <si>
+    <t>Printer state information</t>
+  </si>
+  <si>
+    <t>OS Driver information</t>
+  </si>
+  <si>
+    <t>Import file name</t>
+  </si>
+  <si>
+    <t>Success state of import</t>
+  </si>
+  <si>
+    <t>Save printer configuration request</t>
+  </si>
+  <si>
+    <t>Save material configuration request</t>
+  </si>
+  <si>
+    <t>Loaded printer configuration</t>
+  </si>
+  <si>
+    <t>Loaded material configuration</t>
+  </si>
+  <si>
+    <t>Loaded print configuration</t>
+  </si>
+  <si>
+    <t>Save print configuration request</t>
+  </si>
+  <si>
+    <t>Loaded configuration data</t>
+  </si>
+  <si>
+    <t>Run print job</t>
+  </si>
+  <si>
+    <t>UI21</t>
+  </si>
+  <si>
+    <t>Save print job configuration</t>
+  </si>
+  <si>
+    <t>File Configuration object</t>
+  </si>
+  <si>
+    <t>Printer configuration object</t>
+  </si>
+  <si>
+    <t>Material configuration object</t>
+  </si>
+  <si>
+    <t>Print Configuration object</t>
+  </si>
+  <si>
+    <t>All requested configuration objects</t>
+  </si>
+  <si>
+    <t>Object save/load requests</t>
+  </si>
+  <si>
+    <t>Object save/load results</t>
+  </si>
+  <si>
+    <t>XML File writes to disk</t>
+  </si>
+  <si>
+    <t>UI22</t>
+  </si>
+  <si>
+    <t>Print package object</t>
+  </si>
+  <si>
+    <t>Preprocessing Layer</t>
+  </si>
+  <si>
+    <t>PR1</t>
+  </si>
+  <si>
+    <t>Processing Layer</t>
+  </si>
+  <si>
+    <t>PO1</t>
+  </si>
+  <si>
+    <t>Post-Processing Layer</t>
+  </si>
+  <si>
+    <t>PP1</t>
+  </si>
+  <si>
+    <t>PP2</t>
+  </si>
+  <si>
+    <t>Printer Control Layer</t>
+  </si>
+  <si>
+    <t>PL1</t>
+  </si>
+  <si>
+    <t>G-Code</t>
+  </si>
+  <si>
+    <t>Communications Layer</t>
+  </si>
+  <si>
+    <t>CL1</t>
+  </si>
+  <si>
+    <t>Serialized G-Codes</t>
+  </si>
+  <si>
+    <t>CL2</t>
+  </si>
+  <si>
+    <t>Serialized printer state</t>
+  </si>
+  <si>
+    <t>CL3</t>
+  </si>
+  <si>
+    <t>Command stream</t>
+  </si>
+  <si>
+    <t>Printer Feedback Layer</t>
+  </si>
+  <si>
+    <t>PF1</t>
+  </si>
+  <si>
+    <t>Printer State Object</t>
+  </si>
+  <si>
+    <t>PF2</t>
   </si>
 </sst>
 </file>
@@ -76,15 +289,69 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFED7D31"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB43500"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFAC770D"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF5B9BD5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -92,16 +359,55 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -110,6 +416,17 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF00B050"/>
+      <color rgb="FF7030A0"/>
+      <color rgb="FFA5A5A5"/>
+      <color rgb="FF5B9BD5"/>
+      <color rgb="FFAC770D"/>
+      <color rgb="FFB43500"/>
+      <color rgb="FFED7D31"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -405,89 +722,422 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection sqref="A1:C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6" customWidth="1"/>
-    <col min="3" max="3" width="37.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" customWidth="1"/>
+    <col min="3" max="3" width="40.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:3" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="16" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" t="s">
+      <c r="A3" s="3"/>
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-    </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" t="s">
+      <c r="A5" s="3"/>
+      <c r="B5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" t="s">
+      <c r="A6" s="3"/>
+      <c r="B6" s="4" t="s">
         <v>8</v>
       </c>
+      <c r="C6" s="2" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" t="s">
+      <c r="A7" s="3"/>
+      <c r="B7" s="4" t="s">
         <v>9</v>
       </c>
+      <c r="C7" s="2" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" t="s">
+      <c r="A8" s="3"/>
+      <c r="B8" s="4" t="s">
         <v>10</v>
       </c>
+      <c r="C8" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+      <c r="B13" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="5"/>
+      <c r="B14" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
+      <c r="B15" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="5"/>
+      <c r="B16" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
+      <c r="B17" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="5"/>
+      <c r="B18" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
+      <c r="B19" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="5"/>
+      <c r="B20" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+      <c r="B21" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="5"/>
+      <c r="B22" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="5"/>
+      <c r="B23" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="5"/>
+      <c r="B24" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="5"/>
+      <c r="B25" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="5"/>
+      <c r="B26" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="5"/>
+      <c r="B27" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="5"/>
+      <c r="B28" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="5"/>
+      <c r="B29" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="5"/>
+      <c r="B30" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="5"/>
+      <c r="B31" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="5"/>
+      <c r="B32" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="9"/>
+      <c r="B36" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="12"/>
+      <c r="B39" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="12"/>
+      <c r="B40" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="B41" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="14"/>
+      <c r="B42" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>84</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A2:A8"/>
+  <mergeCells count="5">
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="A38:A40"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="A2:A10"/>
+    <mergeCell ref="A11:A32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>